<commit_message>
Initial Commit with Python3.X support. Initial refactoring for the new "autoaprop" renderer.
</commit_message>
<xml_diff>
--- a/maps/testecadu.xlsx
+++ b/maps/testecadu.xlsx
@@ -11,21 +11,18 @@
     <sheet name="Plan3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$I$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>nome_apropriador</t>
   </si>
   <si>
-    <t>especialidade</t>
-  </si>
-  <si>
     <t>turno</t>
   </si>
   <si>
@@ -66,6 +63,18 @@
   </si>
   <si>
     <t>JULIO</t>
+  </si>
+  <si>
+    <t>nome_setor</t>
+  </si>
+  <si>
+    <t>matr_apropriador</t>
+  </si>
+  <si>
+    <t>nome_planilha</t>
+  </si>
+  <si>
+    <t>flags</t>
   </si>
 </sst>
 </file>
@@ -81,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +100,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,13 +143,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,132 +453,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3621</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4051</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4041</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3930</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3957</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>